<commit_message>
working on multiple files, still broken for "slow" bikes
</commit_message>
<xml_diff>
--- a/bikedef1.xlsx
+++ b/bikedef1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan\Documents\code\triangle-races\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D931EE91-6CD9-42D2-9170-4F3DC6768B98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954C4A44-AC54-4F39-A48D-DDDA3142B230}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19635" yWindow="3960" windowWidth="17700" windowHeight="5085" activeTab="2" xr2:uid="{CF3EC270-673E-4C63-9CCE-0B91219AFD35}"/>
+    <workbookView xWindow="19635" yWindow="3960" windowWidth="17700" windowHeight="5085" xr2:uid="{CF3EC270-673E-4C63-9CCE-0B91219AFD35}"/>
   </bookViews>
   <sheets>
     <sheet name="vehicledyn" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Info</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Ratios</t>
+  </si>
+  <si>
+    <t>Fuel heating value (MJ/kg)</t>
   </si>
 </sst>
 </file>
@@ -480,15 +483,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1027EF2B-558D-425C-8AA2-44CBB5FD91AE}">
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -840,11 +843,19 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>32</v>
+      </c>
+      <c r="B11">
+        <v>50.4</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>25</v>
       </c>
     </row>
@@ -857,9 +868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5DCA7E-AA64-46A5-B806-570C986F4BAD}">
   <dimension ref="A1:V89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8619,7 +8628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE9AA78-FBF9-4F08-BC5C-A2CFB1B47071}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Weight transfer and wheel speed working
</commit_message>
<xml_diff>
--- a/bikedef1.xlsx
+++ b/bikedef1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan\Documents\code\triangle-races\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954C4A44-AC54-4F39-A48D-DDDA3142B230}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4F0D53-4E35-4050-89E4-E205086B3983}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19635" yWindow="3960" windowWidth="17700" windowHeight="5085" xr2:uid="{CF3EC270-673E-4C63-9CCE-0B91219AFD35}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="17700" windowHeight="5085" xr2:uid="{CF3EC270-673E-4C63-9CCE-0B91219AFD35}"/>
   </bookViews>
   <sheets>
     <sheet name="vehicledyn" sheetId="1" r:id="rId1"/>
@@ -485,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1027EF2B-558D-425C-8AA2-44CBB5FD91AE}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3:S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,10 +617,10 @@
         <v>0.41128501861930683</v>
       </c>
       <c r="R3">
-        <v>2.1910929266586197E-2</v>
+        <v>8.9017473503295152E-3</v>
       </c>
       <c r="S3">
-        <v>1.4271632589302385</v>
+        <v>0.57981323403036367</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -652,10 +652,10 @@
         <v>0.41145913855477567</v>
       </c>
       <c r="R4">
-        <v>2.3811016607035797E-2</v>
+        <v>9.6781175597538734E-3</v>
       </c>
       <c r="S4">
-        <v>1.4241726578284892</v>
+        <v>0.57886274388547043</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -687,10 +687,10 @@
         <v>0.41156462585034015</v>
       </c>
       <c r="R5">
-        <v>2.4869952582639521E-2</v>
+        <v>1.0111317254174398E-2</v>
       </c>
       <c r="S5">
-        <v>1.4224548108657702</v>
+        <v>0.57832405689548549</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -722,10 +722,10 @@
         <v>0.40860116032783866</v>
       </c>
       <c r="R6">
-        <v>2.5324194356224662E-2</v>
+        <v>1.0221935721521318E-2</v>
       </c>
       <c r="S6">
-        <v>1.4398287439831878</v>
+        <v>0.58117690395064003</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -757,10 +757,10 @@
         <v>0.4116264687693259</v>
       </c>
       <c r="R7">
-        <v>2.5550319626382784E-2</v>
+        <v>1.038961038961039E-2</v>
       </c>
       <c r="S7">
-        <v>1.4213886144534138</v>
+        <v>0.57798392084106376</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -792,10 +792,10 @@
         <v>0.4116264687693259</v>
       </c>
       <c r="R8">
-        <v>2.5626319548958543E-2</v>
+        <v>1.0420531849103279E-2</v>
       </c>
       <c r="S8">
-        <v>1.421310203826659</v>
+        <v>0.57795299938157074</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -827,10 +827,10 @@
         <v>0.41165739022881881</v>
       </c>
       <c r="R9">
-        <v>2.5700381780550487E-2</v>
+        <v>1.0451453308596165E-2</v>
       </c>
       <c r="S9">
-        <v>1.4210486245464737</v>
+        <v>0.57789115646258504</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>